<commit_message>
dasde - Improved performance..
</commit_message>
<xml_diff>
--- a/dasde 15/Updated File.xlsx
+++ b/dasde 15/Updated File.xlsx
@@ -592,10 +592,8 @@
       <c r="E4" t="n">
         <v>445931234569</v>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>44594</v>
@@ -614,8 +612,10 @@
       <c r="K4" t="n">
         <v>445951234569</v>
       </c>
-      <c r="L4" t="n">
-        <v>0</v>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -756,10 +756,8 @@
       <c r="E8" t="n">
         <v>445951234567</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>44596</v>
@@ -778,8 +776,10 @@
       <c r="K8" t="n">
         <v>445971234567</v>
       </c>
-      <c r="L8" t="n">
-        <v>0</v>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>